<commit_message>
update for Quality Assurance Checklist
</commit_message>
<xml_diff>
--- a/US001 - Quality Assurance Checklist v1.0.xlsx
+++ b/US001 - Quality Assurance Checklist v1.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvo30\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal-my.sharepoint.com/personal/nguyentan_vo_dxc_com/Documents/Desktop/Code/US001/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B34F3A-4E7D-4E14-AF90-5C1C6F4C41D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{75B34F3A-4E7D-4E14-AF90-5C1C6F4C41D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{332F7222-EF50-4373-96B2-053ED8B6387F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -422,19 +422,19 @@
     <t>validator.properties</t>
   </si>
   <si>
-    <t>30/08/2023</t>
-  </si>
-  <si>
     <t>/UserStory001_CreateClient/src/main/resources/messages/validator.properties</t>
   </si>
   <si>
-    <t>log4j.xml</t>
-  </si>
-  <si>
-    <t>26/08/2024</t>
-  </si>
-  <si>
-    <t>/UserStory001_CreateClient/src/main/resources/log4j.xml</t>
+    <t>log4j2.xml</t>
+  </si>
+  <si>
+    <t>30/09/2022</t>
+  </si>
+  <si>
+    <t>30/08/2022</t>
+  </si>
+  <si>
+    <t>/UserStory001_CreateClient/src/main/resources/log4j2.xml</t>
   </si>
 </sst>
 </file>
@@ -1309,7 +1309,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -1928,7 +1928,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="56">
         <v>2</v>
       </c>
@@ -2159,8 +2159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E0A8C1-8EC5-42D2-BAFB-C420B5C8FC7C}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2260,10 +2260,10 @@
         <v>99</v>
       </c>
       <c r="G4" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>102</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>103</v>
       </c>
       <c r="I4" s="25"/>
     </row>
@@ -2275,7 +2275,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>47</v>
@@ -2287,7 +2287,7 @@
         <v>99</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H5" s="19" t="s">
         <v>106</v>
@@ -2533,15 +2533,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068073968EC026B4DBE87DD3E85715D31" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2f7a1f886a19eb4d4656104787b0b142">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c4928f78-8817-462b-a38c-b730d253bc3b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="725f0d8d56db4f087920445967312631" ns2:_="">
     <xsd:import namespace="c4928f78-8817-462b-a38c-b730d253bc3b"/>
@@ -2673,6 +2664,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2680,14 +2680,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB6136B-6A54-49EB-94C3-1CE33ACD540D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C58AD30-BA56-4B7C-9B75-D231FC2808A5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2705,6 +2697,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB6136B-6A54-49EB-94C3-1CE33ACD540D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F67BDBB-3D91-45AE-B771-A0EA7A408106}">
   <ds:schemaRefs>

</xml_diff>